<commit_message>
Adicionada introdução do experimento
</commit_message>
<xml_diff>
--- a/Resources/Data/NTC.xlsx
+++ b/Resources/Data/NTC.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26812"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sheila\Desktop\Instrumentação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Rogiel/Documents/GitHub/ufrgs-instrumentacao-lab4/Resources/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="5445" windowHeight="4635"/>
+    <workbookView xWindow="6400" yWindow="460" windowWidth="25600" windowHeight="14200"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +27,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="3">
+  <si>
+    <t>ref</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -95,9 +108,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -135,14 +148,14 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -175,9 +188,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -207,7 +220,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -357,15 +370,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1">
         <v>16</v>
       </c>
@@ -376,7 +389,7 @@
         <v>3.33</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>18</v>
       </c>
@@ -387,7 +400,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>20</v>
       </c>
@@ -398,7 +411,7 @@
         <v>2.77</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>22</v>
       </c>
@@ -409,7 +422,7 @@
         <v>2.5299999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>24</v>
       </c>
@@ -420,7 +433,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>26</v>
       </c>
@@ -430,8 +443,14 @@
       <c r="C6" s="2">
         <v>2.16</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>28</v>
       </c>
@@ -441,8 +460,11 @@
       <c r="C7" s="1">
         <v>1.97</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>30</v>
       </c>
@@ -453,7 +475,7 @@
         <v>1.77</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>32</v>
       </c>
@@ -464,7 +486,7 @@
         <v>1.64</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>34</v>
       </c>
@@ -475,7 +497,7 @@
         <v>1.52</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>36</v>
       </c>
@@ -486,7 +508,7 @@
         <v>1.38</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>38</v>
       </c>
@@ -497,7 +519,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>40</v>
       </c>
@@ -508,7 +530,7 @@
         <v>1.18</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>42</v>
       </c>
@@ -519,7 +541,7 @@
         <v>1.0900000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>44</v>
       </c>
@@ -529,8 +551,11 @@
       <c r="C15" s="1">
         <v>0.99</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E15" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>46</v>
       </c>
@@ -541,7 +566,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>48</v>
       </c>
@@ -552,7 +577,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>50</v>
       </c>
@@ -563,7 +588,7 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>52</v>
       </c>
@@ -574,7 +599,7 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>54</v>
       </c>
@@ -585,7 +610,7 @@
         <v>0.68</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>56</v>
       </c>
@@ -596,7 +621,7 @@
         <v>0.63</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>58</v>
       </c>
@@ -607,7 +632,7 @@
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>60</v>
       </c>
@@ -617,8 +642,9 @@
       <c r="C23" s="2">
         <v>0.55000000000000004</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>62</v>
       </c>
@@ -628,8 +654,11 @@
       <c r="C24" s="1">
         <v>0.51</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>64</v>
       </c>
@@ -640,7 +669,7 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>66</v>
       </c>
@@ -651,7 +680,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>68</v>
       </c>
@@ -662,7 +691,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>70</v>
       </c>
@@ -673,7 +702,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>72</v>
       </c>
@@ -684,7 +713,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>74</v>
       </c>

</xml_diff>

<commit_message>
Medida feita em 27/04
</commit_message>
<xml_diff>
--- a/Resources/Data/NTC.xlsx
+++ b/Resources/Data/NTC.xlsx
@@ -1,25 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26812"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Rogiel/Documents/GitHub/ufrgs-instrumentacao-lab4/Resources/Data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6400" yWindow="460" windowWidth="25600" windowHeight="14200"/>
+    <workbookView xWindow="6405" yWindow="465" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -27,33 +22,83 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="3">
-  <si>
-    <t>ref</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>-</t>
   </si>
   <si>
-    <t>V</t>
+    <t>3.589 mA</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Imax</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rs</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>R</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vponte</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ponte R2</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ponte R1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ponte R3</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Beta</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>r</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>820//</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vmedido</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Experim.</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="179" formatCode="0.00000000"/>
+    <numFmt numFmtId="181" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -61,17 +106,42 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="新細明體"/>
+      <family val="3"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -86,13 +156,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -105,6 +188,244 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-TW"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Plan1!$A$2:$A$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>44</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Plan1!$M$2:$M$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>-2.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-2.5099999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="0.00">
+                  <c:v>-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-1.52</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-1.1299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="0.00">
+                  <c:v>-0.66</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.11</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.57999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.04</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.71</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.37</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="0.00">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.66</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.3499999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="102569024"/>
+        <c:axId val="102568448"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="102569024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="102568448"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="102568448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="102569024"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="圖表 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -150,7 +471,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -185,7 +506,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -362,7 +683,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -370,15 +691,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:N34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>16</v>
       </c>
@@ -388,19 +714,65 @@
       <c r="C1" s="1">
         <v>3.33</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1">
+        <v>2000</v>
+      </c>
+      <c r="L1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
         <v>18</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="4">
         <v>3</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D2" s="3">
+        <v>467</v>
+      </c>
+      <c r="E2" s="5">
+        <f>1/(1/(C2*1000+$B$33)+1/($B$34))</f>
+        <v>469.90998146677254</v>
+      </c>
+      <c r="F2">
+        <f>$F$1*($I$2*E2-$I$4*$I$2)/(($I$3+$I$4)*($I$2+E2))</f>
+        <v>52.181591701510044</v>
+      </c>
+      <c r="G2" s="7">
+        <f>$F$1*($I$2*D2-$I$4*$I$2)/(($I$3+$I$4)*($I$2+D2))</f>
+        <v>49.087451230922568</v>
+      </c>
+      <c r="H2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="6">
+        <v>530</v>
+      </c>
+      <c r="K2">
+        <v>1500</v>
+      </c>
+      <c r="L2">
+        <v>50.7</v>
+      </c>
+      <c r="M2">
+        <v>-2.8</v>
+      </c>
+      <c r="N2" t="str">
+        <f>CONCATENATE("{",A2,",",M2,"},")</f>
+        <v>{18,-2.8},</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>20</v>
       </c>
@@ -410,8 +782,42 @@
       <c r="C3" s="1">
         <v>2.77</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E3" s="5">
+        <f>1/(1/(C3*1000+$B$33)+1/($B$34))</f>
+        <v>464.7166619678602</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F15" si="0">$F$1*($I$2*E3-$I$4*$I$2)/(($I$3+$I$4)*($I$2+E3))</f>
+        <v>46.646935986311746</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G15" si="1">$F$1*($I$2*D3-$I$4*$I$2)/(($I$3+$I$4)*($I$2+D3))</f>
+        <v>-887.7229800629591</v>
+      </c>
+      <c r="H3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="6">
+        <v>530</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3">
+        <v>1500</v>
+      </c>
+      <c r="L3">
+        <v>43.8</v>
+      </c>
+      <c r="M3">
+        <v>-2.5099999999999998</v>
+      </c>
+      <c r="N3" t="str">
+        <f t="shared" ref="N3:N15" si="2">CONCATENATE("{",A3,",",M3,"},")</f>
+        <v>{20,-2.51},</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>22</v>
       </c>
@@ -421,8 +827,42 @@
       <c r="C4" s="2">
         <v>2.5299999999999998</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E4" s="5">
+        <f>1/(1/(C4*1000+$B$33)+1/($B$34))</f>
+        <v>458.52736619292409</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>39.974890272856101</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="1"/>
+        <v>-887.7229800629591</v>
+      </c>
+      <c r="H4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4">
+        <v>423</v>
+      </c>
+      <c r="J4">
+        <v>390</v>
+      </c>
+      <c r="K4">
+        <v>33</v>
+      </c>
+      <c r="L4">
+        <v>38.1</v>
+      </c>
+      <c r="M4" s="12">
+        <v>-2</v>
+      </c>
+      <c r="N4" t="str">
+        <f t="shared" si="2"/>
+        <v>{22,-2},</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>24</v>
       </c>
@@ -432,8 +872,30 @@
       <c r="C5" s="1">
         <v>2.4</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E5" s="5">
+        <f>1/(1/(C5*1000+$B$33)+1/($B$34))</f>
+        <v>454.78438778722068</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>35.899273553605227</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>-887.7229800629591</v>
+      </c>
+      <c r="L5">
+        <v>31.1</v>
+      </c>
+      <c r="M5">
+        <v>-1.52</v>
+      </c>
+      <c r="N5" t="str">
+        <f t="shared" si="2"/>
+        <v>{24,-1.52},</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>26</v>
       </c>
@@ -443,14 +905,36 @@
       <c r="C6" s="2">
         <v>2.16</v>
       </c>
-      <c r="F6" t="s">
-        <v>2</v>
-      </c>
-      <c r="G6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E6" s="5">
+        <f>1/(1/(C6*1000+$B$33)+1/($B$34))</f>
+        <v>447.00374531835206</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>27.32723844505287</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>-887.7229800629591</v>
+      </c>
+      <c r="H6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6">
+        <v>-8.6680000000000004E-3</v>
+      </c>
+      <c r="L6">
+        <v>23.9</v>
+      </c>
+      <c r="M6">
+        <v>-1.1299999999999999</v>
+      </c>
+      <c r="N6" t="str">
+        <f t="shared" si="2"/>
+        <v>{26,-1.13},</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>28</v>
       </c>
@@ -460,11 +944,37 @@
       <c r="C7" s="1">
         <v>1.97</v>
       </c>
-      <c r="E7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E7" s="5">
+        <f>1/(1/(C7*1000+$B$33)+1/($B$34))</f>
+        <v>439.87986894794318</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>19.35816066654926</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>-887.7229800629591</v>
+      </c>
+      <c r="H7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7">
+        <v>1.2542</v>
+      </c>
+      <c r="L7">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="M7" s="13">
+        <f>-0.66</f>
+        <v>-0.66</v>
+      </c>
+      <c r="N7" t="str">
+        <f t="shared" si="2"/>
+        <v>{28,-0.66},</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>30</v>
       </c>
@@ -474,19 +984,66 @@
       <c r="C8" s="1">
         <v>1.77</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
+      <c r="E8" s="5">
+        <f>1/(1/(C8*1000+$B$33)+1/($B$34))</f>
+        <v>431.232822928936</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>9.526495074485501</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>-887.7229800629591</v>
+      </c>
+      <c r="L8">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="M8">
+        <v>-0.11</v>
+      </c>
+      <c r="N8" t="str">
+        <f t="shared" si="2"/>
+        <v>{30,-0.11},</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
         <v>32</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="4">
         <v>1.65</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="4">
         <v>1.64</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D9" s="3">
+        <v>423</v>
+      </c>
+      <c r="E9" s="5">
+        <f>1/(1/(C9*1000+$B$33)+1/($B$34))</f>
+        <v>424.84484898634673</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>2.149022571516165</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>2.1</v>
+      </c>
+      <c r="M9">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="N9" t="str">
+        <f t="shared" si="2"/>
+        <v>{32,0.58},</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>34</v>
       </c>
@@ -496,8 +1053,30 @@
       <c r="C10" s="1">
         <v>1.52</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E10" s="5">
+        <f>1/(1/(C10*1000+$B$33)+1/($B$34))</f>
+        <v>418.3064867218111</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>-5.5050630098982998</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>-887.7229800629591</v>
+      </c>
+      <c r="L10" s="11">
+        <v>-8</v>
+      </c>
+      <c r="M10">
+        <v>1.04</v>
+      </c>
+      <c r="N10" t="str">
+        <f t="shared" si="2"/>
+        <v>{34,1.04},</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>36</v>
       </c>
@@ -507,8 +1086,30 @@
       <c r="C11" s="1">
         <v>1.38</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E11" s="5">
+        <f>1/(1/(C11*1000+$B$33)+1/($B$34))</f>
+        <v>409.75892443208159</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>-15.671832094966055</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>-887.7229800629591</v>
+      </c>
+      <c r="L11">
+        <v>-15.7</v>
+      </c>
+      <c r="M11">
+        <v>1.71</v>
+      </c>
+      <c r="N11" t="str">
+        <f t="shared" si="2"/>
+        <v>{36,1.71},</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>38</v>
       </c>
@@ -518,8 +1119,30 @@
       <c r="C12" s="2">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E12" s="5">
+        <f>1/(1/(C12*1000+$B$33)+1/($B$34))</f>
+        <v>404.35724602792487</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>-22.192696551164151</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>-887.7229800629591</v>
+      </c>
+      <c r="L12">
+        <v>-23.7</v>
+      </c>
+      <c r="M12">
+        <v>2.37</v>
+      </c>
+      <c r="N12" t="str">
+        <f t="shared" si="2"/>
+        <v>{38,2.37},</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>40</v>
       </c>
@@ -529,8 +1152,30 @@
       <c r="C13" s="2">
         <v>1.18</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E13" s="5">
+        <f>1/(1/(C13*1000+$B$33)+1/($B$34))</f>
+        <v>395.42667347981603</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>-33.140580805065909</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>-887.7229800629591</v>
+      </c>
+      <c r="L13">
+        <v>-36.1</v>
+      </c>
+      <c r="M13" s="12">
+        <v>3</v>
+      </c>
+      <c r="N13" t="str">
+        <f t="shared" si="2"/>
+        <v>{40,3},</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>42</v>
       </c>
@@ -540,22 +1185,66 @@
       <c r="C14" s="1">
         <v>1.0900000000000001</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
+      <c r="E14" s="5">
+        <f>1/(1/(C14*1000+$B$33)+1/($B$34))</f>
+        <v>387.97536154258165</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>-42.438067643041485</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>-887.7229800629591</v>
+      </c>
+      <c r="L14" s="8">
+        <v>-42.9</v>
+      </c>
+      <c r="M14">
+        <v>3.66</v>
+      </c>
+      <c r="N14" t="str">
+        <f t="shared" si="2"/>
+        <v>{42,3.66},</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
         <v>44</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="4">
         <v>1.02</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="4">
         <v>0.99</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D15" s="3">
+        <v>380</v>
+      </c>
+      <c r="E15" s="5">
+        <f>1/(1/(C15*1000+$B$33)+1/($B$34))</f>
+        <v>378.80588568194679</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>-54.088665739169954</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>-52.558144898123913</v>
+      </c>
+      <c r="L15" s="8">
+        <v>-53.9</v>
+      </c>
+      <c r="M15">
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="N15" t="str">
+        <f t="shared" si="2"/>
+        <v>{44,4.35},</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>46</v>
       </c>
@@ -566,7 +1255,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>48</v>
       </c>
@@ -577,7 +1266,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>50</v>
       </c>
@@ -587,8 +1276,15 @@
       <c r="C18" s="1">
         <v>0.79</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="J18">
+        <v>-1.96</v>
+      </c>
+      <c r="K18">
+        <f>-0.2808*J18 + 8.8938</f>
+        <v>9.4441680000000012</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>52</v>
       </c>
@@ -599,7 +1295,7 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>54</v>
       </c>
@@ -610,7 +1306,7 @@
         <v>0.68</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>56</v>
       </c>
@@ -621,7 +1317,7 @@
         <v>0.63</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>58</v>
       </c>
@@ -632,7 +1328,7 @@
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>60</v>
       </c>
@@ -644,7 +1340,7 @@
       </c>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>62</v>
       </c>
@@ -655,10 +1351,10 @@
         <v>0.51</v>
       </c>
       <c r="E24" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>64</v>
       </c>
@@ -669,7 +1365,7 @@
         <v>0.48</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>66</v>
       </c>
@@ -680,7 +1376,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>68</v>
       </c>
@@ -691,7 +1387,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>70</v>
       </c>
@@ -702,7 +1398,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>72</v>
       </c>
@@ -713,7 +1409,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>74</v>
       </c>
@@ -724,8 +1420,46 @@
         <v>0.33</v>
       </c>
     </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>2</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33">
+        <v>227</v>
+      </c>
+      <c r="C33" s="9">
+        <v>180</v>
+      </c>
+      <c r="D33">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34">
+        <v>550</v>
+      </c>
+      <c r="C34">
+        <v>330</v>
+      </c>
+      <c r="D34">
+        <v>220</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adicionado gráficos da resposta temporal do sensor
</commit_message>
<xml_diff>
--- a/Resources/Data/NTC.xlsx
+++ b/Resources/Data/NTC.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26812"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Rogiel/Documents/GitHub/ufrgs-instrumentacao-lab4/Resources/Data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6405" yWindow="465" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19820"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -84,21 +89,21 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="179" formatCode="0.00000000"/>
-    <numFmt numFmtId="181" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.00000000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -106,13 +111,13 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -164,18 +169,18 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -193,7 +198,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="zh-TW"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -236,46 +241,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>18</c:v>
+                  <c:v>18.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>22</c:v>
+                  <c:v>22.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>24</c:v>
+                  <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>26</c:v>
+                  <c:v>26.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>28</c:v>
+                  <c:v>28.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>30</c:v>
+                  <c:v>30.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>34</c:v>
+                  <c:v>34.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>36</c:v>
+                  <c:v>36.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>38</c:v>
+                  <c:v>38.0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>40</c:v>
+                  <c:v>40.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>42</c:v>
+                  <c:v>42.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44</c:v>
+                  <c:v>44.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -290,16 +295,16 @@
                   <c:v>-2.8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-2.5099999999999998</c:v>
+                  <c:v>-2.51</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0.00">
-                  <c:v>-2</c:v>
+                  <c:v>-2.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>-1.52</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-1.1299999999999999</c:v>
+                  <c:v>-1.13</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="0.00">
                   <c:v>-0.66</c:v>
@@ -308,7 +313,7 @@
                   <c:v>-0.11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.57999999999999996</c:v>
+                  <c:v>0.58</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>1.04</c:v>
@@ -320,13 +325,13 @@
                   <c:v>2.37</c:v>
                 </c:pt>
                 <c:pt idx="11" formatCode="0.00">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>3.66</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4.3499999999999996</c:v>
+                  <c:v>4.35</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -341,11 +346,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="102569024"/>
-        <c:axId val="102568448"/>
+        <c:axId val="2111747264"/>
+        <c:axId val="2111734048"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="102569024"/>
+        <c:axId val="2111747264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -355,12 +360,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102568448"/>
+        <c:crossAx val="2111734048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="102568448"/>
+        <c:axId val="2111734048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -371,7 +376,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102569024"/>
+        <c:crossAx val="2111747264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -683,7 +688,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -691,20 +696,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N34"/>
+  <dimension ref="A1:AA34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" s="1">
         <v>16</v>
       </c>
@@ -726,8 +731,16 @@
       <c r="L1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="Z1" t="str">
+        <f>CONCATENATE("{",A1,",",B1*1000,"},")</f>
+        <v>{16,3340},</v>
+      </c>
+      <c r="AA1" t="str">
+        <f>CONCATENATE("{",A1,",",C1*1000,"},")</f>
+        <v>{16,3330},</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>18</v>
       </c>
@@ -768,11 +781,19 @@
         <v>-2.8</v>
       </c>
       <c r="N2" t="str">
-        <f>CONCATENATE("{",A2,",",M2,"},")</f>
-        <v>{18,-2.8},</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+        <f>CONCATENATE("{",A2,",",L2,"},")</f>
+        <v>{18,50.7},</v>
+      </c>
+      <c r="Z2" t="str">
+        <f t="shared" ref="Z2:Z30" si="0">CONCATENATE("{",A2,",",B2*1000,"},")</f>
+        <v>{18,3000},</v>
+      </c>
+      <c r="AA2" t="str">
+        <f t="shared" ref="AA2:AA30" si="1">CONCATENATE("{",A2,",",C2*1000,"},")</f>
+        <v>{18,3000},</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>20</v>
       </c>
@@ -783,15 +804,15 @@
         <v>2.77</v>
       </c>
       <c r="E3" s="5">
-        <f>1/(1/(C3*1000+$B$33)+1/($B$34))</f>
+        <f t="shared" ref="E2:E15" si="2">1/(1/(C3*1000+$B$33)+1/($B$34))</f>
         <v>464.7166619678602</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F15" si="0">$F$1*($I$2*E3-$I$4*$I$2)/(($I$3+$I$4)*($I$2+E3))</f>
+        <f t="shared" ref="F3:F15" si="3">$F$1*($I$2*E3-$I$4*$I$2)/(($I$3+$I$4)*($I$2+E3))</f>
         <v>46.646935986311746</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G15" si="1">$F$1*($I$2*D3-$I$4*$I$2)/(($I$3+$I$4)*($I$2+D3))</f>
+        <f>$F$1*($I$2*D3-$I$4*$I$2)/(($I$3+$I$4)*($I$2+D3))</f>
         <v>-887.7229800629591</v>
       </c>
       <c r="H3" t="s">
@@ -813,11 +834,19 @@
         <v>-2.5099999999999998</v>
       </c>
       <c r="N3" t="str">
-        <f t="shared" ref="N3:N15" si="2">CONCATENATE("{",A3,",",M3,"},")</f>
-        <v>{20,-2.51},</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+        <f t="shared" ref="N3:N15" si="4">CONCATENATE("{",A3,",",L3,"},")</f>
+        <v>{20,43.8},</v>
+      </c>
+      <c r="Z3" t="str">
+        <f t="shared" si="0"/>
+        <v>{20,2810},</v>
+      </c>
+      <c r="AA3" t="str">
+        <f t="shared" si="1"/>
+        <v>{20,2770},</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>22</v>
       </c>
@@ -828,15 +857,15 @@
         <v>2.5299999999999998</v>
       </c>
       <c r="E4" s="5">
-        <f>1/(1/(C4*1000+$B$33)+1/($B$34))</f>
+        <f t="shared" si="2"/>
         <v>458.52736619292409</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>39.974890272856101</v>
       </c>
       <c r="G4">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="G3:G15" si="5">$F$1*($I$2*D4-$I$4*$I$2)/(($I$3+$I$4)*($I$2+D4))</f>
         <v>-887.7229800629591</v>
       </c>
       <c r="H4" t="s">
@@ -858,11 +887,19 @@
         <v>-2</v>
       </c>
       <c r="N4" t="str">
-        <f t="shared" si="2"/>
-        <v>{22,-2},</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>{22,38.1},</v>
+      </c>
+      <c r="Z4" t="str">
+        <f t="shared" si="0"/>
+        <v>{22,2590},</v>
+      </c>
+      <c r="AA4" t="str">
+        <f t="shared" si="1"/>
+        <v>{22,2530},</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>24</v>
       </c>
@@ -873,15 +910,15 @@
         <v>2.4</v>
       </c>
       <c r="E5" s="5">
-        <f>1/(1/(C5*1000+$B$33)+1/($B$34))</f>
+        <f t="shared" si="2"/>
         <v>454.78438778722068</v>
       </c>
       <c r="F5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>35.899273553605227</v>
       </c>
       <c r="G5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>-887.7229800629591</v>
       </c>
       <c r="L5">
@@ -891,11 +928,19 @@
         <v>-1.52</v>
       </c>
       <c r="N5" t="str">
-        <f t="shared" si="2"/>
-        <v>{24,-1.52},</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>{24,31.1},</v>
+      </c>
+      <c r="Z5" t="str">
+        <f t="shared" si="0"/>
+        <v>{24,2380},</v>
+      </c>
+      <c r="AA5" t="str">
+        <f t="shared" si="1"/>
+        <v>{24,2400},</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>26</v>
       </c>
@@ -906,15 +951,15 @@
         <v>2.16</v>
       </c>
       <c r="E6" s="5">
-        <f>1/(1/(C6*1000+$B$33)+1/($B$34))</f>
+        <f t="shared" si="2"/>
         <v>447.00374531835206</v>
       </c>
       <c r="F6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>27.32723844505287</v>
       </c>
       <c r="G6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>-887.7229800629591</v>
       </c>
       <c r="H6" t="s">
@@ -930,11 +975,19 @@
         <v>-1.1299999999999999</v>
       </c>
       <c r="N6" t="str">
-        <f t="shared" si="2"/>
-        <v>{26,-1.13},</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>{26,23.9},</v>
+      </c>
+      <c r="Z6" t="str">
+        <f t="shared" si="0"/>
+        <v>{26,2180},</v>
+      </c>
+      <c r="AA6" t="str">
+        <f t="shared" si="1"/>
+        <v>{26,2160},</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>28</v>
       </c>
@@ -945,15 +998,15 @@
         <v>1.97</v>
       </c>
       <c r="E7" s="5">
-        <f>1/(1/(C7*1000+$B$33)+1/($B$34))</f>
+        <f t="shared" si="2"/>
         <v>439.87986894794318</v>
       </c>
       <c r="F7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>19.35816066654926</v>
       </c>
       <c r="G7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>-887.7229800629591</v>
       </c>
       <c r="H7" t="s">
@@ -970,11 +1023,19 @@
         <v>-0.66</v>
       </c>
       <c r="N7" t="str">
-        <f t="shared" si="2"/>
-        <v>{28,-0.66},</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>{28,18.6},</v>
+      </c>
+      <c r="Z7" t="str">
+        <f t="shared" si="0"/>
+        <v>{28,1990},</v>
+      </c>
+      <c r="AA7" t="str">
+        <f t="shared" si="1"/>
+        <v>{28,1970},</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>30</v>
       </c>
@@ -985,15 +1046,15 @@
         <v>1.77</v>
       </c>
       <c r="E8" s="5">
-        <f>1/(1/(C8*1000+$B$33)+1/($B$34))</f>
+        <f t="shared" si="2"/>
         <v>431.232822928936</v>
       </c>
       <c r="F8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>9.526495074485501</v>
       </c>
       <c r="G8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>-887.7229800629591</v>
       </c>
       <c r="L8">
@@ -1003,11 +1064,19 @@
         <v>-0.11</v>
       </c>
       <c r="N8" t="str">
-        <f t="shared" si="2"/>
-        <v>{30,-0.11},</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>{30,9.8},</v>
+      </c>
+      <c r="Z8" t="str">
+        <f t="shared" si="0"/>
+        <v>{30,1790},</v>
+      </c>
+      <c r="AA8" t="str">
+        <f t="shared" si="1"/>
+        <v>{30,1770},</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>32</v>
       </c>
@@ -1021,15 +1090,15 @@
         <v>423</v>
       </c>
       <c r="E9" s="5">
-        <f>1/(1/(C9*1000+$B$33)+1/($B$34))</f>
+        <f t="shared" si="2"/>
         <v>424.84484898634673</v>
       </c>
       <c r="F9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>2.149022571516165</v>
       </c>
       <c r="G9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L9">
@@ -1039,11 +1108,19 @@
         <v>0.57999999999999996</v>
       </c>
       <c r="N9" t="str">
-        <f t="shared" si="2"/>
-        <v>{32,0.58},</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>{32,2.1},</v>
+      </c>
+      <c r="Z9" t="str">
+        <f t="shared" si="0"/>
+        <v>{32,1650},</v>
+      </c>
+      <c r="AA9" t="str">
+        <f t="shared" si="1"/>
+        <v>{32,1640},</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>34</v>
       </c>
@@ -1054,15 +1131,15 @@
         <v>1.52</v>
       </c>
       <c r="E10" s="5">
-        <f>1/(1/(C10*1000+$B$33)+1/($B$34))</f>
+        <f t="shared" si="2"/>
         <v>418.3064867218111</v>
       </c>
       <c r="F10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-5.5050630098982998</v>
       </c>
       <c r="G10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>-887.7229800629591</v>
       </c>
       <c r="L10" s="11">
@@ -1072,11 +1149,19 @@
         <v>1.04</v>
       </c>
       <c r="N10" t="str">
-        <f t="shared" si="2"/>
-        <v>{34,1.04},</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>{34,-8},</v>
+      </c>
+      <c r="Z10" t="str">
+        <f t="shared" si="0"/>
+        <v>{34,1540},</v>
+      </c>
+      <c r="AA10" t="str">
+        <f t="shared" si="1"/>
+        <v>{34,1520},</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>36</v>
       </c>
@@ -1087,15 +1172,15 @@
         <v>1.38</v>
       </c>
       <c r="E11" s="5">
-        <f>1/(1/(C11*1000+$B$33)+1/($B$34))</f>
+        <f t="shared" si="2"/>
         <v>409.75892443208159</v>
       </c>
       <c r="F11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-15.671832094966055</v>
       </c>
       <c r="G11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>-887.7229800629591</v>
       </c>
       <c r="L11">
@@ -1105,11 +1190,19 @@
         <v>1.71</v>
       </c>
       <c r="N11" t="str">
-        <f t="shared" si="2"/>
-        <v>{36,1.71},</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>{36,-15.7},</v>
+      </c>
+      <c r="Z11" t="str">
+        <f t="shared" si="0"/>
+        <v>{36,1360},</v>
+      </c>
+      <c r="AA11" t="str">
+        <f t="shared" si="1"/>
+        <v>{36,1380},</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>38</v>
       </c>
@@ -1120,15 +1213,15 @@
         <v>1.3</v>
       </c>
       <c r="E12" s="5">
-        <f>1/(1/(C12*1000+$B$33)+1/($B$34))</f>
+        <f t="shared" si="2"/>
         <v>404.35724602792487</v>
       </c>
       <c r="F12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-22.192696551164151</v>
       </c>
       <c r="G12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>-887.7229800629591</v>
       </c>
       <c r="L12">
@@ -1138,11 +1231,19 @@
         <v>2.37</v>
       </c>
       <c r="N12" t="str">
-        <f t="shared" si="2"/>
-        <v>{38,2.37},</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>{38,-23.7},</v>
+      </c>
+      <c r="Z12" t="str">
+        <f t="shared" si="0"/>
+        <v>{38,1310},</v>
+      </c>
+      <c r="AA12" t="str">
+        <f t="shared" si="1"/>
+        <v>{38,1300},</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>40</v>
       </c>
@@ -1153,15 +1254,15 @@
         <v>1.18</v>
       </c>
       <c r="E13" s="5">
-        <f>1/(1/(C13*1000+$B$33)+1/($B$34))</f>
+        <f t="shared" si="2"/>
         <v>395.42667347981603</v>
       </c>
       <c r="F13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-33.140580805065909</v>
       </c>
       <c r="G13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>-887.7229800629591</v>
       </c>
       <c r="L13">
@@ -1171,11 +1272,19 @@
         <v>3</v>
       </c>
       <c r="N13" t="str">
-        <f t="shared" si="2"/>
-        <v>{40,3},</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>{40,-36.1},</v>
+      </c>
+      <c r="Z13" t="str">
+        <f t="shared" si="0"/>
+        <v>{40,1210},</v>
+      </c>
+      <c r="AA13" t="str">
+        <f t="shared" si="1"/>
+        <v>{40,1180},</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>42</v>
       </c>
@@ -1186,15 +1295,15 @@
         <v>1.0900000000000001</v>
       </c>
       <c r="E14" s="5">
-        <f>1/(1/(C14*1000+$B$33)+1/($B$34))</f>
+        <f t="shared" si="2"/>
         <v>387.97536154258165</v>
       </c>
       <c r="F14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-42.438067643041485</v>
       </c>
       <c r="G14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>-887.7229800629591</v>
       </c>
       <c r="L14" s="8">
@@ -1204,11 +1313,19 @@
         <v>3.66</v>
       </c>
       <c r="N14" t="str">
-        <f t="shared" si="2"/>
-        <v>{42,3.66},</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>{42,-42.9},</v>
+      </c>
+      <c r="Z14" t="str">
+        <f t="shared" si="0"/>
+        <v>{42,1110},</v>
+      </c>
+      <c r="AA14" t="str">
+        <f t="shared" si="1"/>
+        <v>{42,1090},</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <v>44</v>
       </c>
@@ -1222,15 +1339,15 @@
         <v>380</v>
       </c>
       <c r="E15" s="5">
-        <f>1/(1/(C15*1000+$B$33)+1/($B$34))</f>
+        <f t="shared" si="2"/>
         <v>378.80588568194679</v>
       </c>
       <c r="F15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>-54.088665739169954</v>
       </c>
       <c r="G15">
-        <f t="shared" si="1"/>
+        <f>$F$1*($I$2*D15-$I$4*$I$2)/(($I$3+$I$4)*($I$2+D15))</f>
         <v>-52.558144898123913</v>
       </c>
       <c r="L15" s="8">
@@ -1240,11 +1357,19 @@
         <v>4.3499999999999996</v>
       </c>
       <c r="N15" t="str">
-        <f t="shared" si="2"/>
-        <v>{44,4.35},</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>{44,-53.9},</v>
+      </c>
+      <c r="Z15" t="str">
+        <f t="shared" si="0"/>
+        <v>{44,1020},</v>
+      </c>
+      <c r="AA15" t="str">
+        <f t="shared" si="1"/>
+        <v>{44,990},</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>46</v>
       </c>
@@ -1254,8 +1379,16 @@
       <c r="C16" s="1">
         <v>0.93</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="Z16" t="str">
+        <f t="shared" si="0"/>
+        <v>{46,950},</v>
+      </c>
+      <c r="AA16" t="str">
+        <f t="shared" si="1"/>
+        <v>{46,930},</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>48</v>
       </c>
@@ -1265,8 +1398,16 @@
       <c r="C17" s="1">
         <v>0.88</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="Z17" t="str">
+        <f t="shared" si="0"/>
+        <v>{48,860},</v>
+      </c>
+      <c r="AA17" t="str">
+        <f t="shared" si="1"/>
+        <v>{48,880},</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>50</v>
       </c>
@@ -1283,8 +1424,16 @@
         <f>-0.2808*J18 + 8.8938</f>
         <v>9.4441680000000012</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="Z18" t="str">
+        <f t="shared" si="0"/>
+        <v>{50,810},</v>
+      </c>
+      <c r="AA18" t="str">
+        <f t="shared" si="1"/>
+        <v>{50,790},</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>52</v>
       </c>
@@ -1294,8 +1443,16 @@
       <c r="C19" s="1">
         <v>0.74</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="Z19" t="str">
+        <f t="shared" si="0"/>
+        <v>{52,740},</v>
+      </c>
+      <c r="AA19" t="str">
+        <f t="shared" si="1"/>
+        <v>{52,740},</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>54</v>
       </c>
@@ -1305,8 +1462,16 @@
       <c r="C20" s="1">
         <v>0.68</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="Z20" t="str">
+        <f t="shared" si="0"/>
+        <v>{54,690},</v>
+      </c>
+      <c r="AA20" t="str">
+        <f t="shared" si="1"/>
+        <v>{54,680},</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>56</v>
       </c>
@@ -1316,8 +1481,16 @@
       <c r="C21" s="1">
         <v>0.63</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="Z21" t="str">
+        <f t="shared" si="0"/>
+        <v>{56,630},</v>
+      </c>
+      <c r="AA21" t="str">
+        <f t="shared" si="1"/>
+        <v>{56,630},</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>58</v>
       </c>
@@ -1327,8 +1500,16 @@
       <c r="C22" s="1">
         <v>0.57999999999999996</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="Z22" t="str">
+        <f t="shared" si="0"/>
+        <v>{58,580},</v>
+      </c>
+      <c r="AA22" t="str">
+        <f t="shared" si="1"/>
+        <v>{58,580},</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>60</v>
       </c>
@@ -1339,8 +1520,16 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="F23" s="2"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="Z23" t="str">
+        <f t="shared" si="0"/>
+        <v>{60,560},</v>
+      </c>
+      <c r="AA23" t="str">
+        <f t="shared" si="1"/>
+        <v>{60,550},</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>62</v>
       </c>
@@ -1353,8 +1542,16 @@
       <c r="E24" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="Z24" t="str">
+        <f t="shared" si="0"/>
+        <v>{62,520},</v>
+      </c>
+      <c r="AA24" t="str">
+        <f t="shared" si="1"/>
+        <v>{62,510},</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>64</v>
       </c>
@@ -1364,8 +1561,16 @@
       <c r="C25" s="1">
         <v>0.48</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="Z25" t="str">
+        <f t="shared" si="0"/>
+        <v>{64,470},</v>
+      </c>
+      <c r="AA25" t="str">
+        <f t="shared" si="1"/>
+        <v>{64,480},</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>66</v>
       </c>
@@ -1375,8 +1580,16 @@
       <c r="C26" s="1">
         <v>0.44</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="Z26" t="str">
+        <f t="shared" si="0"/>
+        <v>{66,460},</v>
+      </c>
+      <c r="AA26" t="str">
+        <f t="shared" si="1"/>
+        <v>{66,440},</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>68</v>
       </c>
@@ -1386,8 +1599,16 @@
       <c r="C27" s="1">
         <v>0.42</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="Z27" t="str">
+        <f t="shared" si="0"/>
+        <v>{68,420},</v>
+      </c>
+      <c r="AA27" t="str">
+        <f t="shared" si="1"/>
+        <v>{68,420},</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>70</v>
       </c>
@@ -1397,8 +1618,16 @@
       <c r="C28" s="1">
         <v>0.38</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="Z28" t="str">
+        <f t="shared" si="0"/>
+        <v>{70,380},</v>
+      </c>
+      <c r="AA28" t="str">
+        <f t="shared" si="1"/>
+        <v>{70,380},</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>72</v>
       </c>
@@ -1408,8 +1637,16 @@
       <c r="C29" s="1">
         <v>0.36</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="Z29" t="str">
+        <f t="shared" si="0"/>
+        <v>{72,360},</v>
+      </c>
+      <c r="AA29" t="str">
+        <f t="shared" si="1"/>
+        <v>{72,360},</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>74</v>
       </c>
@@ -1419,8 +1656,16 @@
       <c r="C30" s="1">
         <v>0.33</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="Z30" t="str">
+        <f t="shared" si="0"/>
+        <v>{74,340},</v>
+      </c>
+      <c r="AA30" t="str">
+        <f t="shared" si="1"/>
+        <v>{74,330},</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>2</v>
       </c>
@@ -1428,7 +1673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>3</v>
       </c>
@@ -1442,7 +1687,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Arrumadas informações sobre o DAQ
</commit_message>
<xml_diff>
--- a/Resources/Data/NTC.xlsx
+++ b/Resources/Data/NTC.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19820"/>
+    <workbookView xWindow="-40" yWindow="460" windowWidth="28800" windowHeight="16240"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -177,7 +177,7 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -346,11 +346,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2111747264"/>
-        <c:axId val="2111734048"/>
+        <c:axId val="2133919424"/>
+        <c:axId val="2133917488"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2111747264"/>
+        <c:axId val="2133919424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -360,12 +360,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2111734048"/>
+        <c:crossAx val="2133917488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2111734048"/>
+        <c:axId val="2133917488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -376,7 +376,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2111747264"/>
+        <c:crossAx val="2133919424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -696,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA34"/>
+  <dimension ref="A1:Z34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -709,7 +709,7 @@
     <col min="14" max="14" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" s="1">
         <v>16</v>
       </c>
@@ -732,15 +732,11 @@
         <v>13</v>
       </c>
       <c r="Z1" t="str">
-        <f>CONCATENATE("{",A1,",",B1*1000,"},")</f>
-        <v>{16,3340},</v>
-      </c>
-      <c r="AA1" t="str">
-        <f>CONCATENATE("{",A1,",",C1*1000,"},")</f>
-        <v>{16,3330},</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
+        <f>CONCATENATE("{",A1,",",B1*1000, ", ", C1*1000,"},")</f>
+        <v>{16,3340, 3330},</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>18</v>
       </c>
@@ -785,15 +781,11 @@
         <v>{18,50.7},</v>
       </c>
       <c r="Z2" t="str">
-        <f t="shared" ref="Z2:Z30" si="0">CONCATENATE("{",A2,",",B2*1000,"},")</f>
-        <v>{18,3000},</v>
-      </c>
-      <c r="AA2" t="str">
-        <f t="shared" ref="AA2:AA30" si="1">CONCATENATE("{",A2,",",C2*1000,"},")</f>
-        <v>{18,3000},</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
+        <f>CONCATENATE("{",A2,",",B2*1000, ", ", C2*1000,"},")</f>
+        <v>{18,3000, 3000},</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>20</v>
       </c>
@@ -804,11 +796,11 @@
         <v>2.77</v>
       </c>
       <c r="E3" s="5">
-        <f t="shared" ref="E2:E15" si="2">1/(1/(C3*1000+$B$33)+1/($B$34))</f>
+        <f t="shared" ref="E3:E15" si="0">1/(1/(C3*1000+$B$33)+1/($B$34))</f>
         <v>464.7166619678602</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F15" si="3">$F$1*($I$2*E3-$I$4*$I$2)/(($I$3+$I$4)*($I$2+E3))</f>
+        <f t="shared" ref="F3:F15" si="1">$F$1*($I$2*E3-$I$4*$I$2)/(($I$3+$I$4)*($I$2+E3))</f>
         <v>46.646935986311746</v>
       </c>
       <c r="G3">
@@ -834,19 +826,15 @@
         <v>-2.5099999999999998</v>
       </c>
       <c r="N3" t="str">
-        <f t="shared" ref="N3:N15" si="4">CONCATENATE("{",A3,",",L3,"},")</f>
+        <f t="shared" ref="N3:N15" si="2">CONCATENATE("{",A3,",",L3,"},")</f>
         <v>{20,43.8},</v>
       </c>
       <c r="Z3" t="str">
-        <f t="shared" si="0"/>
-        <v>{20,2810},</v>
-      </c>
-      <c r="AA3" t="str">
-        <f t="shared" si="1"/>
-        <v>{20,2770},</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+        <f t="shared" ref="Z3:Z30" si="3">CONCATENATE("{",A3,",",B3*1000, ", ", C3*1000,"},")</f>
+        <v>{20,2810, 2770},</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>22</v>
       </c>
@@ -857,15 +845,15 @@
         <v>2.5299999999999998</v>
       </c>
       <c r="E4" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>458.52736619292409</v>
       </c>
       <c r="F4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>39.974890272856101</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G3:G15" si="5">$F$1*($I$2*D4-$I$4*$I$2)/(($I$3+$I$4)*($I$2+D4))</f>
+        <f t="shared" ref="G4:G14" si="4">$F$1*($I$2*D4-$I$4*$I$2)/(($I$3+$I$4)*($I$2+D4))</f>
         <v>-887.7229800629591</v>
       </c>
       <c r="H4" t="s">
@@ -887,19 +875,15 @@
         <v>-2</v>
       </c>
       <c r="N4" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>{22,38.1},</v>
       </c>
       <c r="Z4" t="str">
-        <f t="shared" si="0"/>
-        <v>{22,2590},</v>
-      </c>
-      <c r="AA4" t="str">
-        <f t="shared" si="1"/>
-        <v>{22,2530},</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>{22,2590, 2530},</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>24</v>
       </c>
@@ -910,15 +894,15 @@
         <v>2.4</v>
       </c>
       <c r="E5" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>454.78438778722068</v>
       </c>
       <c r="F5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>35.899273553605227</v>
       </c>
       <c r="G5">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>-887.7229800629591</v>
       </c>
       <c r="L5">
@@ -928,19 +912,15 @@
         <v>-1.52</v>
       </c>
       <c r="N5" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>{24,31.1},</v>
       </c>
       <c r="Z5" t="str">
-        <f t="shared" si="0"/>
-        <v>{24,2380},</v>
-      </c>
-      <c r="AA5" t="str">
-        <f t="shared" si="1"/>
-        <v>{24,2400},</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>{24,2380, 2400},</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>26</v>
       </c>
@@ -951,15 +931,15 @@
         <v>2.16</v>
       </c>
       <c r="E6" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>447.00374531835206</v>
       </c>
       <c r="F6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>27.32723844505287</v>
       </c>
       <c r="G6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>-887.7229800629591</v>
       </c>
       <c r="H6" t="s">
@@ -975,19 +955,15 @@
         <v>-1.1299999999999999</v>
       </c>
       <c r="N6" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>{26,23.9},</v>
       </c>
       <c r="Z6" t="str">
-        <f t="shared" si="0"/>
-        <v>{26,2180},</v>
-      </c>
-      <c r="AA6" t="str">
-        <f t="shared" si="1"/>
-        <v>{26,2160},</v>
-      </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>{26,2180, 2160},</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>28</v>
       </c>
@@ -998,15 +974,15 @@
         <v>1.97</v>
       </c>
       <c r="E7" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>439.87986894794318</v>
       </c>
       <c r="F7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>19.35816066654926</v>
       </c>
       <c r="G7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>-887.7229800629591</v>
       </c>
       <c r="H7" t="s">
@@ -1023,19 +999,15 @@
         <v>-0.66</v>
       </c>
       <c r="N7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>{28,18.6},</v>
       </c>
       <c r="Z7" t="str">
-        <f t="shared" si="0"/>
-        <v>{28,1990},</v>
-      </c>
-      <c r="AA7" t="str">
-        <f t="shared" si="1"/>
-        <v>{28,1970},</v>
-      </c>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>{28,1990, 1970},</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>30</v>
       </c>
@@ -1046,15 +1018,15 @@
         <v>1.77</v>
       </c>
       <c r="E8" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>431.232822928936</v>
       </c>
       <c r="F8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>9.526495074485501</v>
       </c>
       <c r="G8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>-887.7229800629591</v>
       </c>
       <c r="L8">
@@ -1064,19 +1036,15 @@
         <v>-0.11</v>
       </c>
       <c r="N8" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>{30,9.8},</v>
       </c>
       <c r="Z8" t="str">
-        <f t="shared" si="0"/>
-        <v>{30,1790},</v>
-      </c>
-      <c r="AA8" t="str">
-        <f t="shared" si="1"/>
-        <v>{30,1770},</v>
-      </c>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>{30,1790, 1770},</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" s="4">
         <v>32</v>
       </c>
@@ -1090,15 +1058,15 @@
         <v>423</v>
       </c>
       <c r="E9" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>424.84484898634673</v>
       </c>
       <c r="F9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>2.149022571516165</v>
       </c>
       <c r="G9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L9">
@@ -1108,19 +1076,15 @@
         <v>0.57999999999999996</v>
       </c>
       <c r="N9" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>{32,2.1},</v>
       </c>
       <c r="Z9" t="str">
-        <f t="shared" si="0"/>
-        <v>{32,1650},</v>
-      </c>
-      <c r="AA9" t="str">
-        <f t="shared" si="1"/>
-        <v>{32,1640},</v>
-      </c>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>{32,1650, 1640},</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>34</v>
       </c>
@@ -1131,15 +1095,15 @@
         <v>1.52</v>
       </c>
       <c r="E10" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>418.3064867218111</v>
       </c>
       <c r="F10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-5.5050630098982998</v>
       </c>
       <c r="G10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>-887.7229800629591</v>
       </c>
       <c r="L10" s="11">
@@ -1149,19 +1113,15 @@
         <v>1.04</v>
       </c>
       <c r="N10" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>{34,-8},</v>
       </c>
       <c r="Z10" t="str">
-        <f t="shared" si="0"/>
-        <v>{34,1540},</v>
-      </c>
-      <c r="AA10" t="str">
-        <f t="shared" si="1"/>
-        <v>{34,1520},</v>
-      </c>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>{34,1540, 1520},</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>36</v>
       </c>
@@ -1172,15 +1132,15 @@
         <v>1.38</v>
       </c>
       <c r="E11" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>409.75892443208159</v>
       </c>
       <c r="F11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-15.671832094966055</v>
       </c>
       <c r="G11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>-887.7229800629591</v>
       </c>
       <c r="L11">
@@ -1190,19 +1150,15 @@
         <v>1.71</v>
       </c>
       <c r="N11" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>{36,-15.7},</v>
       </c>
       <c r="Z11" t="str">
-        <f t="shared" si="0"/>
-        <v>{36,1360},</v>
-      </c>
-      <c r="AA11" t="str">
-        <f t="shared" si="1"/>
-        <v>{36,1380},</v>
-      </c>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>{36,1360, 1380},</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>38</v>
       </c>
@@ -1213,15 +1169,15 @@
         <v>1.3</v>
       </c>
       <c r="E12" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>404.35724602792487</v>
       </c>
       <c r="F12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-22.192696551164151</v>
       </c>
       <c r="G12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>-887.7229800629591</v>
       </c>
       <c r="L12">
@@ -1231,19 +1187,15 @@
         <v>2.37</v>
       </c>
       <c r="N12" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>{38,-23.7},</v>
       </c>
       <c r="Z12" t="str">
-        <f t="shared" si="0"/>
-        <v>{38,1310},</v>
-      </c>
-      <c r="AA12" t="str">
-        <f t="shared" si="1"/>
-        <v>{38,1300},</v>
-      </c>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>{38,1310, 1300},</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>40</v>
       </c>
@@ -1254,15 +1206,15 @@
         <v>1.18</v>
       </c>
       <c r="E13" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>395.42667347981603</v>
       </c>
       <c r="F13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-33.140580805065909</v>
       </c>
       <c r="G13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>-887.7229800629591</v>
       </c>
       <c r="L13">
@@ -1272,19 +1224,15 @@
         <v>3</v>
       </c>
       <c r="N13" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>{40,-36.1},</v>
       </c>
       <c r="Z13" t="str">
-        <f t="shared" si="0"/>
-        <v>{40,1210},</v>
-      </c>
-      <c r="AA13" t="str">
-        <f t="shared" si="1"/>
-        <v>{40,1180},</v>
-      </c>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>{40,1210, 1180},</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>42</v>
       </c>
@@ -1295,15 +1243,15 @@
         <v>1.0900000000000001</v>
       </c>
       <c r="E14" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>387.97536154258165</v>
       </c>
       <c r="F14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-42.438067643041485</v>
       </c>
       <c r="G14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>-887.7229800629591</v>
       </c>
       <c r="L14" s="8">
@@ -1313,19 +1261,15 @@
         <v>3.66</v>
       </c>
       <c r="N14" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>{42,-42.9},</v>
       </c>
       <c r="Z14" t="str">
-        <f t="shared" si="0"/>
-        <v>{42,1110},</v>
-      </c>
-      <c r="AA14" t="str">
-        <f t="shared" si="1"/>
-        <v>{42,1090},</v>
-      </c>
-    </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>{42,1110, 1090},</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" s="4">
         <v>44</v>
       </c>
@@ -1339,11 +1283,11 @@
         <v>380</v>
       </c>
       <c r="E15" s="5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>378.80588568194679</v>
       </c>
       <c r="F15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>-54.088665739169954</v>
       </c>
       <c r="G15">
@@ -1357,19 +1301,15 @@
         <v>4.3499999999999996</v>
       </c>
       <c r="N15" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>{44,-53.9},</v>
       </c>
       <c r="Z15" t="str">
-        <f t="shared" si="0"/>
-        <v>{44,1020},</v>
-      </c>
-      <c r="AA15" t="str">
-        <f t="shared" si="1"/>
-        <v>{44,990},</v>
-      </c>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>{44,1020, 990},</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>46</v>
       </c>
@@ -1380,15 +1320,11 @@
         <v>0.93</v>
       </c>
       <c r="Z16" t="str">
-        <f t="shared" si="0"/>
-        <v>{46,950},</v>
-      </c>
-      <c r="AA16" t="str">
-        <f t="shared" si="1"/>
-        <v>{46,930},</v>
-      </c>
-    </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>{46,950, 930},</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>48</v>
       </c>
@@ -1399,15 +1335,11 @@
         <v>0.88</v>
       </c>
       <c r="Z17" t="str">
-        <f t="shared" si="0"/>
-        <v>{48,860},</v>
-      </c>
-      <c r="AA17" t="str">
-        <f t="shared" si="1"/>
-        <v>{48,880},</v>
-      </c>
-    </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>{48,860, 880},</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>50</v>
       </c>
@@ -1425,15 +1357,11 @@
         <v>9.4441680000000012</v>
       </c>
       <c r="Z18" t="str">
-        <f t="shared" si="0"/>
-        <v>{50,810},</v>
-      </c>
-      <c r="AA18" t="str">
-        <f t="shared" si="1"/>
-        <v>{50,790},</v>
-      </c>
-    </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>{50,810, 790},</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>52</v>
       </c>
@@ -1444,15 +1372,11 @@
         <v>0.74</v>
       </c>
       <c r="Z19" t="str">
-        <f t="shared" si="0"/>
-        <v>{52,740},</v>
-      </c>
-      <c r="AA19" t="str">
-        <f t="shared" si="1"/>
-        <v>{52,740},</v>
-      </c>
-    </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>{52,740, 740},</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>54</v>
       </c>
@@ -1463,15 +1387,11 @@
         <v>0.68</v>
       </c>
       <c r="Z20" t="str">
-        <f t="shared" si="0"/>
-        <v>{54,690},</v>
-      </c>
-      <c r="AA20" t="str">
-        <f t="shared" si="1"/>
-        <v>{54,680},</v>
-      </c>
-    </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>{54,690, 680},</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>56</v>
       </c>
@@ -1482,15 +1402,11 @@
         <v>0.63</v>
       </c>
       <c r="Z21" t="str">
-        <f t="shared" si="0"/>
-        <v>{56,630},</v>
-      </c>
-      <c r="AA21" t="str">
-        <f t="shared" si="1"/>
-        <v>{56,630},</v>
-      </c>
-    </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>{56,630, 630},</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>58</v>
       </c>
@@ -1501,15 +1417,11 @@
         <v>0.57999999999999996</v>
       </c>
       <c r="Z22" t="str">
-        <f t="shared" si="0"/>
-        <v>{58,580},</v>
-      </c>
-      <c r="AA22" t="str">
-        <f t="shared" si="1"/>
-        <v>{58,580},</v>
-      </c>
-    </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>{58,580, 580},</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>60</v>
       </c>
@@ -1521,15 +1433,11 @@
       </c>
       <c r="F23" s="2"/>
       <c r="Z23" t="str">
-        <f t="shared" si="0"/>
-        <v>{60,560},</v>
-      </c>
-      <c r="AA23" t="str">
-        <f t="shared" si="1"/>
-        <v>{60,550},</v>
-      </c>
-    </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>{60,560, 550},</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>62</v>
       </c>
@@ -1543,15 +1451,11 @@
         <v>0</v>
       </c>
       <c r="Z24" t="str">
-        <f t="shared" si="0"/>
-        <v>{62,520},</v>
-      </c>
-      <c r="AA24" t="str">
-        <f t="shared" si="1"/>
-        <v>{62,510},</v>
-      </c>
-    </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>{62,520, 510},</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>64</v>
       </c>
@@ -1562,15 +1466,11 @@
         <v>0.48</v>
       </c>
       <c r="Z25" t="str">
-        <f t="shared" si="0"/>
-        <v>{64,470},</v>
-      </c>
-      <c r="AA25" t="str">
-        <f t="shared" si="1"/>
-        <v>{64,480},</v>
-      </c>
-    </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>{64,470, 480},</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>66</v>
       </c>
@@ -1581,15 +1481,11 @@
         <v>0.44</v>
       </c>
       <c r="Z26" t="str">
-        <f t="shared" si="0"/>
-        <v>{66,460},</v>
-      </c>
-      <c r="AA26" t="str">
-        <f t="shared" si="1"/>
-        <v>{66,440},</v>
-      </c>
-    </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>{66,460, 440},</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>68</v>
       </c>
@@ -1600,15 +1496,11 @@
         <v>0.42</v>
       </c>
       <c r="Z27" t="str">
-        <f t="shared" si="0"/>
-        <v>{68,420},</v>
-      </c>
-      <c r="AA27" t="str">
-        <f t="shared" si="1"/>
-        <v>{68,420},</v>
-      </c>
-    </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>{68,420, 420},</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>70</v>
       </c>
@@ -1619,15 +1511,11 @@
         <v>0.38</v>
       </c>
       <c r="Z28" t="str">
-        <f t="shared" si="0"/>
-        <v>{70,380},</v>
-      </c>
-      <c r="AA28" t="str">
-        <f t="shared" si="1"/>
-        <v>{70,380},</v>
-      </c>
-    </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>{70,380, 380},</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>72</v>
       </c>
@@ -1638,15 +1526,11 @@
         <v>0.36</v>
       </c>
       <c r="Z29" t="str">
-        <f t="shared" si="0"/>
-        <v>{72,360},</v>
-      </c>
-      <c r="AA29" t="str">
-        <f t="shared" si="1"/>
-        <v>{72,360},</v>
-      </c>
-    </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>{72,360, 360},</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>74</v>
       </c>
@@ -1657,15 +1541,11 @@
         <v>0.33</v>
       </c>
       <c r="Z30" t="str">
-        <f t="shared" si="0"/>
-        <v>{74,340},</v>
-      </c>
-      <c r="AA30" t="str">
-        <f t="shared" si="1"/>
-        <v>{74,330},</v>
-      </c>
-    </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>{74,340, 330},</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>2</v>
       </c>

</xml_diff>